<commit_message>
Import all member data (including profile data), add import id
</commit_message>
<xml_diff>
--- a/src/main/resources/sheets/import-example.xlsx
+++ b/src/main/resources/sheets/import-example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -40,7 +40,13 @@
     <t xml:space="preserve">End Date (yyyy-mm-dd)</t>
   </si>
   <si>
-    <t xml:space="preserve">MEMBERS =&gt;</t>
+    <t xml:space="preserve">Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UniqueNum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEMBERS=&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Member Name</t>
@@ -55,39 +61,39 @@
     <t xml:space="preserve">Role</t>
   </si>
   <si>
+    <t xml:space="preserve">Position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City</t>
+  </si>
+  <si>
     <t xml:space="preserve">Date of birth</t>
   </si>
   <si>
     <t xml:space="preserve">Sex</t>
   </si>
   <si>
-    <t xml:space="preserve">Country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone</t>
+    <t xml:space="preserve">Phone Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">About me</t>
   </si>
   <si>
     <t xml:space="preserve">Social Networks</t>
   </si>
   <si>
-    <t xml:space="preserve">About me</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tools</t>
-  </si>
-  <si>
     <t xml:space="preserve">6Hands webapp</t>
   </si>
   <si>
@@ -100,6 +106,12 @@
     <t xml:space="preserve">Web Development</t>
   </si>
   <si>
+    <t xml:space="preserve">projLnk1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Peter(Member)</t>
   </si>
   <si>
@@ -112,6 +124,33 @@
     <t xml:space="preserve">Frontend developer</t>
   </si>
   <si>
+    <t xml:space="preserve">Junior Developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frontend development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web development1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDE1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russia1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moscow1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cool info about me1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">socials1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Phil(Member)</t>
   </si>
   <si>
@@ -121,6 +160,33 @@
     <t xml:space="preserve">Backend developer</t>
   </si>
   <si>
+    <t xml:space="preserve">Middle Developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web development2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDE2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russia2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moscow2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cool info about me2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">socials2</t>
+  </si>
+  <si>
     <t xml:space="preserve">6Hands webapp2</t>
   </si>
   <si>
@@ -133,6 +199,12 @@
     <t xml:space="preserve">Web Development 2</t>
   </si>
   <si>
+    <t xml:space="preserve">projLnk2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Peter(Member)2</t>
   </si>
   <si>
@@ -145,6 +217,30 @@
     <t xml:space="preserve">Frontend developer2</t>
   </si>
   <si>
+    <t xml:space="preserve">Junior Developer2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frontend development2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web development3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russia3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moscow3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cool info about me3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">socials3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Phil(Member)2</t>
   </si>
   <si>
@@ -152,6 +248,30 @@
   </si>
   <si>
     <t xml:space="preserve">Backend developer2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middle Developer2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend development2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web development4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDE4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russia4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moscow4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cool info about me4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">socials4</t>
   </si>
 </sst>
 </file>
@@ -189,7 +309,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF999999"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -282,66 +402,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF999999"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -350,27 +410,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O14" activeCellId="0" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="12.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,22 +458,22 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="4" t="s">
@@ -432,30 +495,33 @@
         <v>18</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>44058</v>
@@ -463,45 +529,117 @@
       <c r="F2" s="5" t="n">
         <v>44084</v>
       </c>
+      <c r="G2" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="H2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>30</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="T2" s="5" t="n">
+        <v>33151</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>32</v>
+      <c r="L3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="T3" s="5" t="n">
+        <v>33152</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="V3" s="0" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>44059</v>
@@ -509,39 +647,111 @@
       <c r="F4" s="5" t="n">
         <v>44085</v>
       </c>
+      <c r="G4" s="0" t="s">
+        <v>59</v>
+      </c>
       <c r="H4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>39</v>
+        <v>60</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>61</v>
       </c>
       <c r="K4" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="T4" s="5" t="n">
+        <v>33153</v>
+      </c>
+      <c r="U4" s="0" t="s">
         <v>40</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="X4" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>42</v>
+      <c r="J5" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>43</v>
+        <v>62</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="T5" s="5" t="n">
+        <v>33154</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="X5" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" display="test2@sixhands.dev"/>
-    <hyperlink ref="J3" r:id="rId2" display="test3@sixhands.dev"/>
-    <hyperlink ref="J4" r:id="rId3" display="test2@sixhands.dev2"/>
-    <hyperlink ref="J5" r:id="rId4" display="test3@sixhands.dev2"/>
+    <hyperlink ref="L2" r:id="rId1" display="test2@sixhands.dev"/>
+    <hyperlink ref="L3" r:id="rId2" display="test3@sixhands.dev"/>
+    <hyperlink ref="L4" r:id="rId3" display="test2@sixhands.dev2"/>
+    <hyperlink ref="L5" r:id="rId4" display="test3@sixhands.dev2"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>